<commit_message>
Added a new way to calculate the field using numpy so the calculations are roungly 45 times faster than the previous itteration
</commit_message>
<xml_diff>
--- a/locations.xlsx
+++ b/locations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Number</t>
   </si>
@@ -46,6 +46,12 @@
   <si>
     <t>adjusted x-0.07 and y-0.04</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
 </sst>
 </file>
 
@@ -60,12 +66,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -89,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -98,6 +110,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -417,7 +432,7 @@
   <dimension ref="C7:L96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,6 +476,12 @@
       <c r="I8" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="J8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
@@ -488,11 +509,11 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K9">
-        <v>4.5000000000000005E-2</v>
+        <v>-4.5000000000000005E-2</v>
       </c>
       <c r="L9">
         <f>K9*-1</f>
-        <v>-4.5000000000000005E-2</v>
+        <v>4.5000000000000005E-2</v>
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.25">
@@ -521,11 +542,11 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K10">
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="L10">
         <f t="shared" ref="L10:L73" si="0">K10*-1</f>
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.25">
@@ -554,11 +575,11 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K11">
+        <v>4.9999999999999975E-3</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
         <v>-4.9999999999999975E-3</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="0"/>
-        <v>4.9999999999999975E-3</v>
       </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
@@ -587,11 +608,11 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
         <v>-1.4999999999999999E-2</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
@@ -620,11 +641,11 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K13">
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
         <v>-2.4999999999999994E-2</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="0"/>
-        <v>2.4999999999999994E-2</v>
       </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
@@ -653,11 +674,11 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K14">
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
@@ -686,11 +707,11 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K15">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
         <v>-4.4999999999999998E-2</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="0"/>
-        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
@@ -719,11 +740,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K16">
+        <v>-4.5000000000000005E-2</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
         <v>4.5000000000000005E-2</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="0"/>
-        <v>-4.5000000000000005E-2</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.25">
@@ -752,11 +773,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K17">
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.25">
@@ -785,11 +806,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K18">
+        <v>-2.0000000000000004E-2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
         <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="0"/>
-        <v>-2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
@@ -818,11 +839,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K19">
+        <v>-1.0000000000000002E-2</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
         <v>1.0000000000000002E-2</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="0"/>
-        <v>-1.0000000000000002E-2</v>
       </c>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.25">
@@ -884,11 +905,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K21">
+        <v>9.999999999999995E-3</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
         <v>-9.999999999999995E-3</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="0"/>
-        <v>9.999999999999995E-3</v>
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
@@ -917,11 +938,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K22">
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
         <v>-2.4999999999999994E-2</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="0"/>
-        <v>2.4999999999999994E-2</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
@@ -950,11 +971,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K23">
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
@@ -983,11 +1004,11 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="K24">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
         <v>-4.4999999999999998E-2</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="0"/>
-        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.25">
@@ -1016,11 +1037,11 @@
         <v>2.4999999999999994E-2</v>
       </c>
       <c r="K25">
+        <v>-4.5000000000000005E-2</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
         <v>4.5000000000000005E-2</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="0"/>
-        <v>-4.5000000000000005E-2</v>
       </c>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.25">
@@ -1049,11 +1070,11 @@
         <v>2.4999999999999994E-2</v>
       </c>
       <c r="K26">
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="L26">
         <f t="shared" si="0"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
@@ -1082,11 +1103,11 @@
         <v>2.4999999999999994E-2</v>
       </c>
       <c r="K27">
+        <v>-2.0000000000000004E-2</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
         <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="0"/>
-        <v>-2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
@@ -1115,11 +1136,11 @@
         <v>2.4999999999999994E-2</v>
       </c>
       <c r="K28">
+        <v>-1.0000000000000002E-2</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
         <v>1.0000000000000002E-2</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="0"/>
-        <v>-1.0000000000000002E-2</v>
       </c>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.25">
@@ -1181,11 +1202,11 @@
         <v>2.4999999999999994E-2</v>
       </c>
       <c r="K30">
+        <v>9.999999999999995E-3</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
         <v>-9.999999999999995E-3</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="0"/>
-        <v>9.999999999999995E-3</v>
       </c>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.25">
@@ -1214,11 +1235,11 @@
         <v>2.4999999999999994E-2</v>
       </c>
       <c r="K31">
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
         <v>-2.4999999999999994E-2</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="0"/>
-        <v>2.4999999999999994E-2</v>
       </c>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.25">
@@ -1247,11 +1268,11 @@
         <v>2.4999999999999994E-2</v>
       </c>
       <c r="K32">
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
@@ -1280,11 +1301,11 @@
         <v>2.4999999999999994E-2</v>
       </c>
       <c r="K33">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
         <v>-4.4999999999999998E-2</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="0"/>
-        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
@@ -1313,11 +1334,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K34">
+        <v>-4.5000000000000005E-2</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
         <v>4.5000000000000005E-2</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="0"/>
-        <v>-4.5000000000000005E-2</v>
       </c>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.25">
@@ -1346,11 +1367,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K35">
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.25">
@@ -1379,11 +1400,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K36">
+        <v>-2.0000000000000004E-2</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="0"/>
         <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="0"/>
-        <v>-2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.25">
@@ -1412,11 +1433,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K37">
+        <v>-1.0000000000000002E-2</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="0"/>
         <v>1.0000000000000002E-2</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="0"/>
-        <v>-1.0000000000000002E-2</v>
       </c>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
@@ -1478,11 +1499,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K39">
+        <v>9.999999999999995E-3</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="0"/>
         <v>-9.999999999999995E-3</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="0"/>
-        <v>9.999999999999995E-3</v>
       </c>
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.25">
@@ -1511,11 +1532,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K40">
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="0"/>
         <v>-2.4999999999999994E-2</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="0"/>
-        <v>2.4999999999999994E-2</v>
       </c>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
@@ -1544,11 +1565,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K41">
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L41">
         <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
@@ -1577,11 +1598,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K42">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="0"/>
         <v>-4.4999999999999998E-2</v>
-      </c>
-      <c r="L42">
-        <f t="shared" si="0"/>
-        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
@@ -1610,11 +1631,11 @@
         <v>4.9999999999999975E-3</v>
       </c>
       <c r="K43">
+        <v>-4.5000000000000005E-2</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="0"/>
         <v>4.5000000000000005E-2</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="0"/>
-        <v>-4.5000000000000005E-2</v>
       </c>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
@@ -1643,11 +1664,11 @@
         <v>4.9999999999999975E-3</v>
       </c>
       <c r="K44">
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="L44">
         <f t="shared" si="0"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
@@ -1676,11 +1697,11 @@
         <v>4.9999999999999975E-3</v>
       </c>
       <c r="K45">
+        <v>-2.0000000000000004E-2</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="0"/>
         <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="L45">
-        <f t="shared" si="0"/>
-        <v>-2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="46" spans="3:12" x14ac:dyDescent="0.25">
@@ -1709,11 +1730,11 @@
         <v>4.9999999999999975E-3</v>
       </c>
       <c r="K46">
+        <v>-1.0000000000000002E-2</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="0"/>
         <v>1.0000000000000002E-2</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="0"/>
-        <v>-1.0000000000000002E-2</v>
       </c>
     </row>
     <row r="47" spans="3:12" x14ac:dyDescent="0.25">
@@ -1775,11 +1796,11 @@
         <v>4.9999999999999975E-3</v>
       </c>
       <c r="K48">
+        <v>9.999999999999995E-3</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="0"/>
         <v>-9.999999999999995E-3</v>
-      </c>
-      <c r="L48">
-        <f t="shared" si="0"/>
-        <v>9.999999999999995E-3</v>
       </c>
     </row>
     <row r="49" spans="3:12" x14ac:dyDescent="0.25">
@@ -1808,11 +1829,11 @@
         <v>4.9999999999999975E-3</v>
       </c>
       <c r="K49">
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="0"/>
         <v>-2.4999999999999994E-2</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="0"/>
-        <v>2.4999999999999994E-2</v>
       </c>
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.25">
@@ -1841,11 +1862,11 @@
         <v>4.9999999999999975E-3</v>
       </c>
       <c r="K50">
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L50">
         <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.25">
@@ -1874,11 +1895,11 @@
         <v>4.9999999999999975E-3</v>
       </c>
       <c r="K51">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="0"/>
         <v>-4.4999999999999998E-2</v>
-      </c>
-      <c r="L51">
-        <f t="shared" si="0"/>
-        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.25">
@@ -1907,11 +1928,11 @@
         <v>-5.0000000000000044E-3</v>
       </c>
       <c r="K52">
+        <v>-4.5000000000000005E-2</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="0"/>
         <v>4.5000000000000005E-2</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="0"/>
-        <v>-4.5000000000000005E-2</v>
       </c>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.25">
@@ -1940,11 +1961,11 @@
         <v>-5.0000000000000044E-3</v>
       </c>
       <c r="K53">
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="L53">
         <f t="shared" si="0"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="54" spans="3:12" x14ac:dyDescent="0.25">
@@ -1973,11 +1994,11 @@
         <v>-5.0000000000000044E-3</v>
       </c>
       <c r="K54">
+        <v>-2.0000000000000004E-2</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="0"/>
         <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="L54">
-        <f t="shared" si="0"/>
-        <v>-2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="55" spans="3:12" x14ac:dyDescent="0.25">
@@ -2006,11 +2027,11 @@
         <v>-5.0000000000000044E-3</v>
       </c>
       <c r="K55">
+        <v>-1.0000000000000002E-2</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="0"/>
         <v>1.0000000000000002E-2</v>
-      </c>
-      <c r="L55">
-        <f t="shared" si="0"/>
-        <v>-1.0000000000000002E-2</v>
       </c>
     </row>
     <row r="56" spans="3:12" x14ac:dyDescent="0.25">
@@ -2072,11 +2093,11 @@
         <v>-5.0000000000000044E-3</v>
       </c>
       <c r="K57">
+        <v>9.999999999999995E-3</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="0"/>
         <v>-9.999999999999995E-3</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="0"/>
-        <v>9.999999999999995E-3</v>
       </c>
     </row>
     <row r="58" spans="3:12" x14ac:dyDescent="0.25">
@@ -2105,11 +2126,11 @@
         <v>-5.0000000000000044E-3</v>
       </c>
       <c r="K58">
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="0"/>
         <v>-2.4999999999999994E-2</v>
-      </c>
-      <c r="L58">
-        <f t="shared" si="0"/>
-        <v>2.4999999999999994E-2</v>
       </c>
     </row>
     <row r="59" spans="3:12" x14ac:dyDescent="0.25">
@@ -2138,11 +2159,11 @@
         <v>-5.0000000000000044E-3</v>
       </c>
       <c r="K59">
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L59">
         <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="60" spans="3:12" x14ac:dyDescent="0.25">
@@ -2171,11 +2192,11 @@
         <v>-5.0000000000000044E-3</v>
       </c>
       <c r="K60">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="0"/>
         <v>-4.4999999999999998E-2</v>
-      </c>
-      <c r="L60">
-        <f t="shared" si="0"/>
-        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="61" spans="3:12" x14ac:dyDescent="0.25">
@@ -2204,11 +2225,11 @@
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="K61">
+        <v>-4.5000000000000005E-2</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="0"/>
         <v>4.5000000000000005E-2</v>
-      </c>
-      <c r="L61">
-        <f t="shared" si="0"/>
-        <v>-4.5000000000000005E-2</v>
       </c>
     </row>
     <row r="62" spans="3:12" x14ac:dyDescent="0.25">
@@ -2237,11 +2258,11 @@
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="K62">
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="L62">
         <f t="shared" si="0"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="63" spans="3:12" x14ac:dyDescent="0.25">
@@ -2270,11 +2291,11 @@
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="K63">
+        <v>-2.0000000000000004E-2</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="0"/>
         <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="L63">
-        <f t="shared" si="0"/>
-        <v>-2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.25">
@@ -2303,11 +2324,11 @@
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="K64">
+        <v>-1.0000000000000002E-2</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="0"/>
         <v>1.0000000000000002E-2</v>
-      </c>
-      <c r="L64">
-        <f t="shared" si="0"/>
-        <v>-1.0000000000000002E-2</v>
       </c>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.25">
@@ -2369,11 +2390,11 @@
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="K66">
+        <v>9.999999999999995E-3</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="0"/>
         <v>-9.999999999999995E-3</v>
-      </c>
-      <c r="L66">
-        <f t="shared" si="0"/>
-        <v>9.999999999999995E-3</v>
       </c>
     </row>
     <row r="67" spans="3:12" x14ac:dyDescent="0.25">
@@ -2402,11 +2423,11 @@
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="K67">
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="0"/>
         <v>-2.4999999999999994E-2</v>
-      </c>
-      <c r="L67">
-        <f t="shared" si="0"/>
-        <v>2.4999999999999994E-2</v>
       </c>
     </row>
     <row r="68" spans="3:12" x14ac:dyDescent="0.25">
@@ -2435,11 +2456,11 @@
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="K68">
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L68">
         <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="69" spans="3:12" x14ac:dyDescent="0.25">
@@ -2468,11 +2489,11 @@
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="K69">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="0"/>
         <v>-4.4999999999999998E-2</v>
-      </c>
-      <c r="L69">
-        <f t="shared" si="0"/>
-        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="70" spans="3:12" x14ac:dyDescent="0.25">
@@ -2501,11 +2522,11 @@
         <v>-2.5000000000000001E-2</v>
       </c>
       <c r="K70">
+        <v>-4.5000000000000005E-2</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="0"/>
         <v>4.5000000000000005E-2</v>
-      </c>
-      <c r="L70">
-        <f t="shared" si="0"/>
-        <v>-4.5000000000000005E-2</v>
       </c>
     </row>
     <row r="71" spans="3:12" x14ac:dyDescent="0.25">
@@ -2534,11 +2555,11 @@
         <v>-2.5000000000000001E-2</v>
       </c>
       <c r="K71">
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="L71">
         <f t="shared" si="0"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="72" spans="3:12" x14ac:dyDescent="0.25">
@@ -2567,11 +2588,11 @@
         <v>-2.5000000000000001E-2</v>
       </c>
       <c r="K72">
+        <v>-2.0000000000000004E-2</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="0"/>
         <v>2.0000000000000004E-2</v>
-      </c>
-      <c r="L72">
-        <f t="shared" si="0"/>
-        <v>-2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="73" spans="3:12" x14ac:dyDescent="0.25">
@@ -2600,11 +2621,11 @@
         <v>-2.5000000000000001E-2</v>
       </c>
       <c r="K73">
+        <v>-1.0000000000000002E-2</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="0"/>
         <v>1.0000000000000002E-2</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="0"/>
-        <v>-1.0000000000000002E-2</v>
       </c>
     </row>
     <row r="74" spans="3:12" x14ac:dyDescent="0.25">
@@ -2666,11 +2687,11 @@
         <v>-2.5000000000000001E-2</v>
       </c>
       <c r="K75">
-        <v>-9.999999999999995E-3</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="L75">
         <f t="shared" si="1"/>
-        <v>9.999999999999995E-3</v>
+        <v>-9.999999999999995E-3</v>
       </c>
     </row>
     <row r="76" spans="3:12" x14ac:dyDescent="0.25">
@@ -2699,11 +2720,11 @@
         <v>-2.5000000000000001E-2</v>
       </c>
       <c r="K76">
-        <v>-2.4999999999999994E-2</v>
+        <v>2.4999999999999994E-2</v>
       </c>
       <c r="L76">
         <f t="shared" si="1"/>
-        <v>2.4999999999999994E-2</v>
+        <v>-2.4999999999999994E-2</v>
       </c>
     </row>
     <row r="77" spans="3:12" x14ac:dyDescent="0.25">
@@ -2732,11 +2753,11 @@
         <v>-2.5000000000000001E-2</v>
       </c>
       <c r="K77">
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L77">
         <f t="shared" si="1"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="78" spans="3:12" x14ac:dyDescent="0.25">
@@ -2765,11 +2786,11 @@
         <v>-2.5000000000000001E-2</v>
       </c>
       <c r="K78">
-        <v>-4.4999999999999998E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="L78">
         <f t="shared" si="1"/>
-        <v>4.4999999999999998E-2</v>
+        <v>-4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="79" spans="3:12" x14ac:dyDescent="0.25">
@@ -2798,11 +2819,11 @@
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="K79">
-        <v>4.5000000000000005E-2</v>
+        <v>-4.5000000000000005E-2</v>
       </c>
       <c r="L79">
         <f t="shared" si="1"/>
-        <v>-4.5000000000000005E-2</v>
+        <v>4.5000000000000005E-2</v>
       </c>
     </row>
     <row r="80" spans="3:12" x14ac:dyDescent="0.25">
@@ -2831,11 +2852,11 @@
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="K80">
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="L80">
         <f t="shared" si="1"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="81" spans="3:12" x14ac:dyDescent="0.25">
@@ -2864,11 +2885,11 @@
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="K81">
-        <v>2.0000000000000004E-2</v>
+        <v>-2.0000000000000004E-2</v>
       </c>
       <c r="L81">
         <f t="shared" si="1"/>
-        <v>-2.0000000000000004E-2</v>
+        <v>2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="82" spans="3:12" x14ac:dyDescent="0.25">
@@ -2897,11 +2918,11 @@
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="K82">
-        <v>1.0000000000000002E-2</v>
+        <v>-1.0000000000000002E-2</v>
       </c>
       <c r="L82">
         <f t="shared" si="1"/>
-        <v>-1.0000000000000002E-2</v>
+        <v>1.0000000000000002E-2</v>
       </c>
     </row>
     <row r="83" spans="3:12" x14ac:dyDescent="0.25">
@@ -2963,11 +2984,11 @@
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="K84">
-        <v>-9.999999999999995E-3</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="L84">
         <f t="shared" si="1"/>
-        <v>9.999999999999995E-3</v>
+        <v>-9.999999999999995E-3</v>
       </c>
     </row>
     <row r="85" spans="3:12" x14ac:dyDescent="0.25">
@@ -2996,11 +3017,11 @@
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="K85">
-        <v>-2.4999999999999994E-2</v>
+        <v>2.4999999999999994E-2</v>
       </c>
       <c r="L85">
         <f t="shared" si="1"/>
-        <v>2.4999999999999994E-2</v>
+        <v>-2.4999999999999994E-2</v>
       </c>
     </row>
     <row r="86" spans="3:12" x14ac:dyDescent="0.25">
@@ -3029,11 +3050,11 @@
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="K86">
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L86">
         <f t="shared" si="1"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="87" spans="3:12" x14ac:dyDescent="0.25">
@@ -3062,11 +3083,11 @@
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="K87">
-        <v>-4.4999999999999998E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="L87">
         <f t="shared" si="1"/>
-        <v>4.4999999999999998E-2</v>
+        <v>-4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="88" spans="3:12" x14ac:dyDescent="0.25">
@@ -3095,11 +3116,11 @@
         <v>-4.5000000000000005E-2</v>
       </c>
       <c r="K88">
-        <v>4.5000000000000005E-2</v>
+        <v>-4.5000000000000005E-2</v>
       </c>
       <c r="L88">
         <f t="shared" si="1"/>
-        <v>-4.5000000000000005E-2</v>
+        <v>4.5000000000000005E-2</v>
       </c>
     </row>
     <row r="89" spans="3:12" x14ac:dyDescent="0.25">
@@ -3128,11 +3149,11 @@
         <v>-4.5000000000000005E-2</v>
       </c>
       <c r="K89">
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="L89">
         <f t="shared" si="1"/>
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="90" spans="3:12" x14ac:dyDescent="0.25">
@@ -3161,11 +3182,11 @@
         <v>-4.5000000000000005E-2</v>
       </c>
       <c r="K90">
-        <v>2.0000000000000004E-2</v>
+        <v>-2.0000000000000004E-2</v>
       </c>
       <c r="L90">
         <f t="shared" si="1"/>
-        <v>-2.0000000000000004E-2</v>
+        <v>2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="91" spans="3:12" x14ac:dyDescent="0.25">
@@ -3194,11 +3215,11 @@
         <v>-4.5000000000000005E-2</v>
       </c>
       <c r="K91">
-        <v>1.0000000000000002E-2</v>
+        <v>-1.0000000000000002E-2</v>
       </c>
       <c r="L91">
         <f t="shared" si="1"/>
-        <v>-1.0000000000000002E-2</v>
+        <v>1.0000000000000002E-2</v>
       </c>
     </row>
     <row r="92" spans="3:12" x14ac:dyDescent="0.25">
@@ -3260,11 +3281,11 @@
         <v>-4.5000000000000005E-2</v>
       </c>
       <c r="K93">
-        <v>-9.999999999999995E-3</v>
+        <v>9.999999999999995E-3</v>
       </c>
       <c r="L93">
         <f t="shared" si="1"/>
-        <v>9.999999999999995E-3</v>
+        <v>-9.999999999999995E-3</v>
       </c>
     </row>
     <row r="94" spans="3:12" x14ac:dyDescent="0.25">
@@ -3293,11 +3314,11 @@
         <v>-4.5000000000000005E-2</v>
       </c>
       <c r="K94">
-        <v>-2.4999999999999994E-2</v>
+        <v>2.4999999999999994E-2</v>
       </c>
       <c r="L94">
         <f t="shared" si="1"/>
-        <v>2.4999999999999994E-2</v>
+        <v>-2.4999999999999994E-2</v>
       </c>
     </row>
     <row r="95" spans="3:12" x14ac:dyDescent="0.25">
@@ -3326,11 +3347,11 @@
         <v>-4.5000000000000005E-2</v>
       </c>
       <c r="K95">
-        <v>-3.5000000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="L95">
         <f t="shared" si="1"/>
-        <v>3.5000000000000003E-2</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="96" spans="3:12" x14ac:dyDescent="0.25">
@@ -3359,11 +3380,11 @@
         <v>-4.5000000000000005E-2</v>
       </c>
       <c r="K96">
-        <v>-4.4999999999999998E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="L96">
         <f t="shared" si="1"/>
-        <v>4.4999999999999998E-2</v>
+        <v>-4.4999999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>